<commit_message>
New table for Aim1
</commit_message>
<xml_diff>
--- a/data-clean/overall_temp_table.xlsx
+++ b/data-clean/overall_temp_table.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samharper/git/bhet-report/data-clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B405CF10-7890-D949-A2C0-6D8DF51B4A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89453118-5BD6-8849-B6EE-ED77474D089F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="760" windowWidth="20100" windowHeight="11560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="760" windowWidth="27980" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -49,9 +49,6 @@
     <t>ci</t>
   </si>
   <si>
-    <t xml:space="preserve"> (0, 1.29)</t>
-  </si>
-  <si>
     <t>(-0.08, 1.72)</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>(2.19, 5.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (0.00, 1.29)</t>
   </si>
 </sst>
 </file>
@@ -108,11 +108,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +421,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -443,66 +444,66 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.64</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0.82</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1.8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1.85</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>3.83</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>3.72</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>